<commit_message>
fixed more DC subnets
</commit_message>
<xml_diff>
--- a/example_Input_Enterprise_networks-v1.xlsx
+++ b/example_Input_Enterprise_networks-v1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC48793A-38F2-4887-A519-C9D0838D5257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A4C0DA-23BD-4A9F-89FF-B1185E5E562E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41145" yWindow="1755" windowWidth="13815" windowHeight="11385" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application_identifier (2)" sheetId="19" r:id="rId1"/>
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="340">
   <si>
     <t>Please do not delete any of these rows!</t>
   </si>
@@ -1019,9 +1019,6 @@
     <t>172.21.149.0/24</t>
   </si>
   <si>
-    <t>172.22.0.0/16</t>
-  </si>
-  <si>
     <t>Insight_Australia</t>
   </si>
   <si>
@@ -1169,9 +1166,6 @@
     <t>172.20.0.0/16</t>
   </si>
   <si>
-    <t>172.16.6.0/16</t>
-  </si>
-  <si>
     <t>SAP ?</t>
   </si>
   <si>
@@ -1365,6 +1359,78 @@
   </si>
   <si>
     <t>PMVS_central_qa</t>
+  </si>
+  <si>
+    <t>10.250.0.0/16</t>
+  </si>
+  <si>
+    <t>10.120.0.0/16</t>
+  </si>
+  <si>
+    <t>10.117.0.0/16</t>
+  </si>
+  <si>
+    <t>10.113.0.0/16</t>
+  </si>
+  <si>
+    <t>10.119.0.0/16</t>
+  </si>
+  <si>
+    <t>10.53.0.0/16</t>
+  </si>
+  <si>
+    <t>10.241.9.24</t>
+  </si>
+  <si>
+    <t>Symantec</t>
+  </si>
+  <si>
+    <t>10.109.0.0/16</t>
+  </si>
+  <si>
+    <t>10.100.0.0/16</t>
+  </si>
+  <si>
+    <t>10.107.0.0/16</t>
+  </si>
+  <si>
+    <t>10.11.0.0/16</t>
+  </si>
+  <si>
+    <t>10.133.0.0/16</t>
+  </si>
+  <si>
+    <t>10.135.0.0/16</t>
+  </si>
+  <si>
+    <t>10.145.0.0/16</t>
+  </si>
+  <si>
+    <t>10.146.0.0/16</t>
+  </si>
+  <si>
+    <t>172.25.9.27</t>
+  </si>
+  <si>
+    <t>172.25.52.32</t>
+  </si>
+  <si>
+    <t>172.25.52.31</t>
+  </si>
+  <si>
+    <t>172.25.52.29</t>
+  </si>
+  <si>
+    <t>SAP_external</t>
+  </si>
+  <si>
+    <t>104.80.112.63</t>
+  </si>
+  <si>
+    <t>172.25.52.21</t>
+  </si>
+  <si>
+    <t>ecpascs</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D4A65C-B460-4641-8F46-FF0C318459A7}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
@@ -2278,7 +2344,7 @@
         <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2357,26 +2423,26 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2440,7 +2506,7 @@
         <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2448,7 +2514,7 @@
         <v>118</v>
       </c>
       <c r="B56" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2456,7 +2522,7 @@
         <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2464,7 +2530,7 @@
         <v>120</v>
       </c>
       <c r="B58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2472,7 +2538,7 @@
         <v>121</v>
       </c>
       <c r="B59" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2480,7 +2546,7 @@
         <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2488,7 +2554,7 @@
         <v>123</v>
       </c>
       <c r="B61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2496,7 +2562,7 @@
         <v>124</v>
       </c>
       <c r="B62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,7 +2732,7 @@
         <v>58</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -2674,13 +2740,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B82" t="s">
         <v>162</v>
       </c>
       <c r="C82" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2691,7 +2757,7 @@
         <v>162</v>
       </c>
       <c r="C83" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,7 +2768,7 @@
         <v>162</v>
       </c>
       <c r="C84" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2713,73 +2779,73 @@
         <v>162</v>
       </c>
       <c r="C85" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B86" t="s">
         <v>162</v>
       </c>
       <c r="C86" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B87" t="s">
         <v>162</v>
       </c>
       <c r="C87" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B88" t="s">
         <v>162</v>
       </c>
       <c r="C88" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B89" t="s">
         <v>162</v>
       </c>
       <c r="C89" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B90" t="s">
         <v>162</v>
       </c>
       <c r="C90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B91" t="s">
         <v>162</v>
       </c>
       <c r="C91" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2859,7 +2925,7 @@
         <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -2867,10 +2933,10 @@
         <v>129</v>
       </c>
       <c r="B102" t="s">
+        <v>234</v>
+      </c>
+      <c r="G102" t="s">
         <v>235</v>
-      </c>
-      <c r="G102" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -2998,7 +3064,7 @@
         <v>92</v>
       </c>
       <c r="B118" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -3006,47 +3072,47 @@
         <v>95</v>
       </c>
       <c r="B119" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B121" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B122" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B123" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -3086,15 +3152,15 @@
         <v>89</v>
       </c>
       <c r="B129" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B130" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -3102,7 +3168,7 @@
         <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -3110,7 +3176,7 @@
         <v>125</v>
       </c>
       <c r="B132" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -3118,7 +3184,7 @@
         <v>67</v>
       </c>
       <c r="B133" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -3126,15 +3192,15 @@
         <v>69</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B135" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3142,7 +3208,7 @@
         <v>63</v>
       </c>
       <c r="B136" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3150,7 +3216,7 @@
         <v>64</v>
       </c>
       <c r="B137" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -3158,7 +3224,7 @@
         <v>65</v>
       </c>
       <c r="B138" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3166,28 +3232,28 @@
         <v>68</v>
       </c>
       <c r="B139" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B150" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B151" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3249,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D842548-09A4-4220-AFD0-E2D7704A9209}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3274,7 +3340,7 @@
         <v>186</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3282,7 +3348,7 @@
         <v>186</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,7 +3356,7 @@
         <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3298,7 +3364,7 @@
         <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3306,7 +3372,7 @@
         <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3314,7 +3380,7 @@
         <v>186</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3322,7 +3388,7 @@
         <v>186</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3330,127 +3396,121 @@
         <v>186</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" t="s">
-        <v>212</v>
+      <c r="A10" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" t="s">
-        <v>213</v>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" t="s">
-        <v>214</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B16" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" t="s">
         <v>203</v>
-      </c>
-      <c r="B17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B18" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>209</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>202</v>
+      </c>
+      <c r="B19" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>202</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>199</v>
+      <c r="A21" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>200</v>
+        <v>208</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3458,7 +3518,7 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -3466,7 +3526,7 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3474,7 +3534,7 @@
         <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3482,79 +3542,183 @@
         <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>227</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>228</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>316</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>316</v>
+        <v>226</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>194</v>
+        <v>314</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>315</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B35" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>316</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>4</v>
+        <v>314</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>314</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>314</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>314</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>314</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>314</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>314</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>314</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>314</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>314</v>
+      </c>
+      <c r="B47" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>314</v>
+      </c>
+      <c r="B48" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>314</v>
+      </c>
+      <c r="B49" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>314</v>
+      </c>
+      <c r="B50" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3566,10 +3730,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B44"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,242 +3856,250 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>249</v>
+      </c>
+      <c r="B45" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3942,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3973,7 +4145,7 @@
         <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,26 +4224,26 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4135,7 +4307,7 @@
         <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4143,7 +4315,7 @@
         <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -4151,7 +4323,7 @@
         <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4159,7 +4331,7 @@
         <v>120</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -4167,7 +4339,7 @@
         <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -4175,7 +4347,7 @@
         <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -4183,7 +4355,7 @@
         <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -4191,7 +4363,7 @@
         <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -4343,258 +4515,273 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>237</v>
+        <v>337</v>
       </c>
       <c r="B47" t="s">
         <v>162</v>
       </c>
       <c r="C47" t="s">
-        <v>238</v>
+        <v>336</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>236</v>
       </c>
       <c r="B48" t="s">
         <v>162</v>
       </c>
       <c r="C48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
         <v>162</v>
       </c>
       <c r="C49" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>335</v>
       </c>
       <c r="B50" t="s">
         <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>239</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>240</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
         <v>162</v>
       </c>
       <c r="C51" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>242</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
         <v>162</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>243</v>
+        <v>334</v>
       </c>
       <c r="B53" t="s">
         <v>162</v>
       </c>
       <c r="C53" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>244</v>
+        <v>333</v>
       </c>
       <c r="B54" t="s">
         <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>246</v>
+        <v>338</v>
       </c>
       <c r="B55" t="s">
         <v>162</v>
       </c>
       <c r="C55" t="s">
-        <v>245</v>
+        <v>339</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B56" t="s">
         <v>162</v>
       </c>
       <c r="C56" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>241</v>
       </c>
       <c r="B57" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="C57" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="B58" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="B59" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="C59" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>245</v>
       </c>
       <c r="B60" t="s">
-        <v>191</v>
+        <v>162</v>
+      </c>
+      <c r="C60" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>247</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="C61" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B65" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>164</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="B70" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>165</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B74" t="s">
         <v>165</v>
@@ -4602,7 +4789,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B75" t="s">
         <v>165</v>
@@ -4610,7 +4797,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
         <v>165</v>
@@ -4618,7 +4805,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B77" t="s">
         <v>165</v>
@@ -4626,7 +4813,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B78" t="s">
         <v>165</v>
@@ -4634,7 +4821,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B79" t="s">
         <v>165</v>
@@ -4642,7 +4829,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
         <v>165</v>
@@ -4650,7 +4837,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B81" t="s">
         <v>165</v>
@@ -4658,7 +4845,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B82" t="s">
         <v>165</v>
@@ -4666,178 +4853,178 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="B84" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="B85" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="B86" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>179</v>
       </c>
       <c r="B87" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>220</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>216</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>217</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>218</v>
       </c>
       <c r="B92" t="s">
-        <v>87</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>128</v>
+        <v>219</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>89</v>
+        <v>220</v>
       </c>
       <c r="B94" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>224</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
-        <v>223</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>226</v>
+        <v>88</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="B97" t="s">
-        <v>226</v>
+        <v>87</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>67</v>
+        <v>128</v>
       </c>
       <c r="B98" t="s">
-        <v>229</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B99" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B100" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>125</v>
       </c>
       <c r="B102" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>65</v>
+        <v>322</v>
       </c>
       <c r="B103" t="s">
-        <v>229</v>
+        <v>323</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>68</v>
+        <v>332</v>
       </c>
       <c r="B104" t="s">
-        <v>229</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>